<commit_message>
ACF - Editar datos desde el excel
</commit_message>
<xml_diff>
--- a/docs/Mapeo-caracteristicas-activos.xlsx
+++ b/docs/Mapeo-caracteristicas-activos.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacho\Documents\GitHub\Prueba\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="251">
   <si>
     <t>Columna(s) of "acfCRSt_Caracteristicas" Table</t>
   </si>
@@ -774,13 +769,16 @@
   </si>
   <si>
     <t>ACFSaldoGravable</t>
+  </si>
+  <si>
+    <t>clase contable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1071,6 +1069,13 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1080,12 +1085,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1182,7 +1183,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1359,32 +1360,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93:M115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
       <c r="H1" t="s">
         <v>161</v>
       </c>
@@ -1403,8 +1404,12 @@
       <c r="M1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N1" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="23.25" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1486,7 +1491,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="23.25" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1519,7 +1524,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="23.25" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1560,7 +1565,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1593,7 +1598,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1628,7 +1633,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1665,7 +1670,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="23.25" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1696,7 +1701,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1725,7 +1730,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="34.5" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1795,7 +1800,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>40</v>
       </c>
@@ -1826,7 +1831,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
@@ -1857,7 +1862,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>46</v>
       </c>
@@ -1888,7 +1893,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>49</v>
       </c>
@@ -1919,7 +1924,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>51</v>
       </c>
@@ -1950,7 +1955,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>53</v>
       </c>
@@ -1981,7 +1986,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>55</v>
       </c>
@@ -2012,7 +2017,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
@@ -2043,7 +2048,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>60</v>
       </c>
@@ -2074,7 +2079,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" s="13" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="13" customFormat="1" ht="23.25" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2110,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>65</v>
       </c>
@@ -2136,7 +2141,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>67</v>
       </c>
@@ -2167,7 +2172,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A25" s="14" t="s">
         <v>69</v>
       </c>
@@ -2198,7 +2203,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="14" t="s">
         <v>72</v>
       </c>
@@ -2229,7 +2234,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A27" s="14" t="s">
         <v>74</v>
       </c>
@@ -2260,7 +2265,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -2291,7 +2296,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A29" s="14" t="s">
         <v>78</v>
       </c>
@@ -2322,7 +2327,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" s="18" customFormat="1" ht="23.25" thickBot="1">
       <c r="A30" s="14" t="s">
         <v>80</v>
       </c>
@@ -2353,7 +2358,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A31" s="14" t="s">
         <v>82</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A32" s="14" t="s">
         <v>84</v>
       </c>
@@ -2415,7 +2420,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" s="18" customFormat="1" ht="23.25" thickBot="1">
       <c r="A33" s="14" t="s">
         <v>86</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A34" s="14" t="s">
         <v>88</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A35" s="14" t="s">
         <v>91</v>
       </c>
@@ -2508,7 +2513,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" s="23" customFormat="1" ht="15.75" thickBot="1">
       <c r="A36" s="19" t="s">
         <v>93</v>
       </c>
@@ -2539,7 +2544,7 @@
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
     </row>
-    <row r="37" spans="1:13" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" s="23" customFormat="1" ht="15.75" thickBot="1">
       <c r="A37" s="19" t="s">
         <v>95</v>
       </c>
@@ -2570,7 +2575,7 @@
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
     </row>
-    <row r="38" spans="1:13" s="23" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" s="23" customFormat="1" ht="23.25" thickBot="1">
       <c r="A38" s="19" t="s">
         <v>97</v>
       </c>
@@ -2601,7 +2606,7 @@
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
     </row>
-    <row r="39" spans="1:13" s="23" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" s="23" customFormat="1" ht="23.25" thickBot="1">
       <c r="A39" s="19" t="s">
         <v>99</v>
       </c>
@@ -2632,7 +2637,7 @@
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
     </row>
-    <row r="40" spans="1:13" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" s="23" customFormat="1" ht="15.75" thickBot="1">
       <c r="A40" s="19" t="s">
         <v>101</v>
       </c>
@@ -2663,7 +2668,7 @@
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
     </row>
-    <row r="41" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="23.25" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>103</v>
       </c>
@@ -2696,7 +2701,7 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="23.25" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>106</v>
       </c>
@@ -2729,7 +2734,7 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="15.75" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -2762,7 +2767,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
     </row>
-    <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="15.75" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>110</v>
       </c>
@@ -2795,7 +2800,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
     </row>
-    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="23.25" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>113</v>
       </c>
@@ -2828,7 +2833,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="23.25" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>115</v>
       </c>
@@ -2861,7 +2866,7 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
     </row>
-    <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="15.75" thickBot="1">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
@@ -2894,7 +2899,7 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
     </row>
-    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="15.75" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>119</v>
       </c>
@@ -2927,7 +2932,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="15.75" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>122</v>
       </c>
@@ -2960,7 +2965,7 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
     </row>
-    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="23.25" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>124</v>
       </c>
@@ -2991,7 +2996,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="15.75" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>126</v>
       </c>
@@ -3022,7 +3027,7 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
-    <row r="52" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="34.5" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>128</v>
       </c>
@@ -3053,7 +3058,7 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
     </row>
-    <row r="53" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="23.25" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>130</v>
       </c>
@@ -3084,7 +3089,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
     </row>
-    <row r="54" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="23.25" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>132</v>
       </c>
@@ -3115,7 +3120,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="23.25" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
@@ -3146,7 +3151,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="23.25" thickBot="1">
       <c r="A56" s="3" t="s">
         <v>136</v>
       </c>
@@ -3177,7 +3182,7 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
     </row>
-    <row r="57" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="34.5" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>138</v>
       </c>
@@ -3208,7 +3213,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
     </row>
-    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="23.25" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>140</v>
       </c>
@@ -3239,7 +3244,7 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
-    <row r="59" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" ht="23.25" thickBot="1">
       <c r="A59" s="3" t="s">
         <v>142</v>
       </c>
@@ -3270,7 +3275,7 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
     </row>
-    <row r="60" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="15.75" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
@@ -3301,7 +3306,7 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="15.75" thickBot="1">
       <c r="A61" s="3" t="s">
         <v>148</v>
       </c>
@@ -3332,7 +3337,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="23.25" thickBot="1">
       <c r="A62" s="3" t="s">
         <v>150</v>
       </c>
@@ -3363,7 +3368,7 @@
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="15.75" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>152</v>
       </c>
@@ -3394,7 +3399,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="15.75" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>154</v>
       </c>
@@ -3425,7 +3430,7 @@
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
     </row>
-    <row r="65" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" ht="34.5" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>156</v>
       </c>
@@ -3456,7 +3461,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
     </row>
-    <row r="66" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" ht="23.25" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>158</v>
       </c>
@@ -3487,25 +3492,25 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="68" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="24" t="s">
+    <row r="68" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="69" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A69" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-    </row>
-    <row r="70" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
+      <c r="M69" s="25"/>
+    </row>
+    <row r="70" spans="1:13" ht="15.75" thickBot="1">
       <c r="A70" s="1" t="s">
         <v>1</v>
       </c>
@@ -3524,17 +3529,17 @@
       <c r="F70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G70" s="27" t="s">
+      <c r="G70" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
-      <c r="K70" s="28"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="28"/>
-    </row>
-    <row r="71" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="25"/>
+      <c r="I70" s="25"/>
+      <c r="J70" s="25"/>
+      <c r="K70" s="25"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="25"/>
+    </row>
+    <row r="71" spans="1:13" ht="34.5" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>175</v>
       </c>
@@ -3556,16 +3561,16 @@
       <c r="G71" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
-      <c r="M71" s="28"/>
-    </row>
-    <row r="72" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H71" s="25"/>
+      <c r="I71" s="25"/>
+      <c r="J71" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K71" s="25"/>
+      <c r="L71" s="25"/>
+      <c r="M71" s="25"/>
+    </row>
+    <row r="72" spans="1:13" ht="15.75" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>177</v>
       </c>
@@ -3587,16 +3592,16 @@
       <c r="G72" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K72" s="28"/>
-      <c r="L72" s="28"/>
-      <c r="M72" s="28"/>
-    </row>
-    <row r="73" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H72" s="25"/>
+      <c r="I72" s="25"/>
+      <c r="J72" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K72" s="25"/>
+      <c r="L72" s="25"/>
+      <c r="M72" s="25"/>
+    </row>
+    <row r="73" spans="1:13" ht="34.5" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>180</v>
       </c>
@@ -3618,16 +3623,16 @@
       <c r="G73" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
-    </row>
-    <row r="74" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H73" s="25"/>
+      <c r="I73" s="25"/>
+      <c r="J73" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K73" s="25"/>
+      <c r="L73" s="25"/>
+      <c r="M73" s="25"/>
+    </row>
+    <row r="74" spans="1:13" ht="34.5" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>183</v>
       </c>
@@ -3649,16 +3654,16 @@
       <c r="G74" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K74" s="28"/>
-      <c r="L74" s="28"/>
-      <c r="M74" s="28"/>
-    </row>
-    <row r="75" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H74" s="25"/>
+      <c r="I74" s="25"/>
+      <c r="J74" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K74" s="25"/>
+      <c r="L74" s="25"/>
+      <c r="M74" s="25"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.75" thickBot="1">
       <c r="A75" s="3" t="s">
         <v>186</v>
       </c>
@@ -3680,16 +3685,16 @@
       <c r="G75" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
-      <c r="M75" s="28"/>
-    </row>
-    <row r="76" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H75" s="25"/>
+      <c r="I75" s="25"/>
+      <c r="J75" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K75" s="25"/>
+      <c r="L75" s="25"/>
+      <c r="M75" s="25"/>
+    </row>
+    <row r="76" spans="1:13" ht="34.5" thickBot="1">
       <c r="A76" s="3" t="s">
         <v>188</v>
       </c>
@@ -3711,16 +3716,16 @@
       <c r="G76" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="28"/>
-    </row>
-    <row r="77" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H76" s="25"/>
+      <c r="I76" s="25"/>
+      <c r="J76" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K76" s="25"/>
+      <c r="L76" s="25"/>
+      <c r="M76" s="25"/>
+    </row>
+    <row r="77" spans="1:13" ht="15.75" thickBot="1">
       <c r="A77" s="3" t="s">
         <v>190</v>
       </c>
@@ -3742,16 +3747,16 @@
       <c r="G77" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
-      <c r="M77" s="28"/>
-    </row>
-    <row r="78" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H77" s="25"/>
+      <c r="I77" s="25"/>
+      <c r="J77" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K77" s="25"/>
+      <c r="L77" s="25"/>
+      <c r="M77" s="25"/>
+    </row>
+    <row r="78" spans="1:13" ht="15.75" thickBot="1">
       <c r="A78" s="3" t="s">
         <v>192</v>
       </c>
@@ -3773,16 +3778,16 @@
       <c r="G78" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K78" s="28"/>
-      <c r="L78" s="28"/>
-      <c r="M78" s="28"/>
-    </row>
-    <row r="79" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H78" s="25"/>
+      <c r="I78" s="25"/>
+      <c r="J78" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K78" s="25"/>
+      <c r="L78" s="25"/>
+      <c r="M78" s="25"/>
+    </row>
+    <row r="79" spans="1:13" ht="23.25" thickBot="1">
       <c r="A79" s="3" t="s">
         <v>194</v>
       </c>
@@ -3804,16 +3809,16 @@
       <c r="G79" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="28"/>
-    </row>
-    <row r="80" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H79" s="25"/>
+      <c r="I79" s="25"/>
+      <c r="J79" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K79" s="25"/>
+      <c r="L79" s="25"/>
+      <c r="M79" s="25"/>
+    </row>
+    <row r="80" spans="1:13" ht="23.25" thickBot="1">
       <c r="A80" s="3" t="s">
         <v>196</v>
       </c>
@@ -3835,16 +3840,16 @@
       <c r="G80" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K80" s="28"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="28"/>
-    </row>
-    <row r="81" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H80" s="25"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K80" s="25"/>
+      <c r="L80" s="25"/>
+      <c r="M80" s="25"/>
+    </row>
+    <row r="81" spans="1:13" ht="15.75" thickBot="1">
       <c r="A81" s="3" t="s">
         <v>198</v>
       </c>
@@ -3866,16 +3871,16 @@
       <c r="G81" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K81" s="28"/>
-      <c r="L81" s="28"/>
-      <c r="M81" s="28"/>
-    </row>
-    <row r="82" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H81" s="25"/>
+      <c r="I81" s="25"/>
+      <c r="J81" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K81" s="25"/>
+      <c r="L81" s="25"/>
+      <c r="M81" s="25"/>
+    </row>
+    <row r="82" spans="1:13" ht="15.75" thickBot="1">
       <c r="A82" s="3" t="s">
         <v>200</v>
       </c>
@@ -3897,16 +3902,16 @@
       <c r="G82" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H82" s="28"/>
-      <c r="I82" s="28"/>
-      <c r="J82" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K82" s="28"/>
-      <c r="L82" s="28"/>
-      <c r="M82" s="28"/>
-    </row>
-    <row r="83" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H82" s="25"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K82" s="25"/>
+      <c r="L82" s="25"/>
+      <c r="M82" s="25"/>
+    </row>
+    <row r="83" spans="1:13" ht="15.75" thickBot="1">
       <c r="A83" s="3" t="s">
         <v>202</v>
       </c>
@@ -3928,16 +3933,16 @@
       <c r="G83" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-      <c r="J83" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K83" s="28"/>
-      <c r="L83" s="28"/>
-      <c r="M83" s="28"/>
-    </row>
-    <row r="84" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H83" s="25"/>
+      <c r="I83" s="25"/>
+      <c r="J83" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K83" s="25"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="25"/>
+    </row>
+    <row r="84" spans="1:13" ht="23.25" thickBot="1">
       <c r="A84" s="3" t="s">
         <v>205</v>
       </c>
@@ -3959,16 +3964,16 @@
       <c r="G84" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-      <c r="J84" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K84" s="28"/>
-      <c r="L84" s="28"/>
-      <c r="M84" s="28"/>
-    </row>
-    <row r="85" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H84" s="25"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K84" s="25"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+    </row>
+    <row r="85" spans="1:13" ht="15.75" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>207</v>
       </c>
@@ -3990,16 +3995,16 @@
       <c r="G85" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H85" s="28"/>
-      <c r="I85" s="28"/>
-      <c r="J85" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K85" s="28"/>
-      <c r="L85" s="28"/>
-      <c r="M85" s="28"/>
-    </row>
-    <row r="86" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H85" s="25"/>
+      <c r="I85" s="25"/>
+      <c r="J85" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K85" s="25"/>
+      <c r="L85" s="25"/>
+      <c r="M85" s="25"/>
+    </row>
+    <row r="86" spans="1:13" ht="23.25" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>209</v>
       </c>
@@ -4021,16 +4026,16 @@
       <c r="G86" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K86" s="28"/>
-      <c r="L86" s="28"/>
-      <c r="M86" s="28"/>
-    </row>
-    <row r="87" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H86" s="25"/>
+      <c r="I86" s="25"/>
+      <c r="J86" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K86" s="25"/>
+      <c r="L86" s="25"/>
+      <c r="M86" s="25"/>
+    </row>
+    <row r="87" spans="1:13" ht="15.75" thickBot="1">
       <c r="A87" s="3" t="s">
         <v>211</v>
       </c>
@@ -4052,16 +4057,16 @@
       <c r="G87" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-      <c r="J87" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K87" s="28"/>
-      <c r="L87" s="28"/>
-      <c r="M87" s="28"/>
-    </row>
-    <row r="88" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H87" s="25"/>
+      <c r="I87" s="25"/>
+      <c r="J87" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K87" s="25"/>
+      <c r="L87" s="25"/>
+      <c r="M87" s="25"/>
+    </row>
+    <row r="88" spans="1:13" ht="23.25" thickBot="1">
       <c r="A88" s="3" t="s">
         <v>213</v>
       </c>
@@ -4083,16 +4088,16 @@
       <c r="G88" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H88" s="28"/>
-      <c r="I88" s="28"/>
-      <c r="J88" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K88" s="28"/>
-      <c r="L88" s="28"/>
-      <c r="M88" s="28"/>
-    </row>
-    <row r="89" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="25"/>
+    </row>
+    <row r="89" spans="1:13" ht="23.25" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>8</v>
       </c>
@@ -4114,28 +4119,28 @@
       <c r="G89" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H89" s="28"/>
-      <c r="I89" s="28"/>
-      <c r="J89" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="K89" s="28"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="28"/>
-    </row>
-    <row r="90" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="91" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="24" t="s">
+      <c r="H89" s="25"/>
+      <c r="I89" s="25"/>
+      <c r="J89" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K89" s="25"/>
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
+    </row>
+    <row r="90" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="91" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A91" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="26"/>
-    </row>
-    <row r="92" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="29"/>
+    </row>
+    <row r="92" spans="1:13" ht="15.75" thickBot="1">
       <c r="A92" s="1" t="s">
         <v>1</v>
       </c>
@@ -4158,7 +4163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" ht="15.75" thickBot="1">
       <c r="A93" s="3" t="s">
         <v>216</v>
       </c>
@@ -4178,16 +4183,16 @@
       <c r="G93" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H93" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="28"/>
-    </row>
-    <row r="94" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H93" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I93" s="25"/>
+      <c r="J93" s="25"/>
+      <c r="K93" s="25"/>
+      <c r="L93" s="25"/>
+      <c r="M93" s="25"/>
+    </row>
+    <row r="94" spans="1:13" ht="23.25" thickBot="1">
       <c r="A94" s="3" t="s">
         <v>124</v>
       </c>
@@ -4209,16 +4214,16 @@
       <c r="G94" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H94" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="28"/>
-    </row>
-    <row r="95" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H94" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I94" s="25"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="25"/>
+      <c r="M94" s="25"/>
+    </row>
+    <row r="95" spans="1:13" ht="23.25" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>103</v>
       </c>
@@ -4240,16 +4245,16 @@
       <c r="G95" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H95" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
-      <c r="K95" s="28"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="28"/>
-    </row>
-    <row r="96" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H95" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I95" s="25"/>
+      <c r="J95" s="25"/>
+      <c r="K95" s="25"/>
+      <c r="L95" s="25"/>
+      <c r="M95" s="25"/>
+    </row>
+    <row r="96" spans="1:13" ht="23.25" thickBot="1">
       <c r="A96" s="3" t="s">
         <v>115</v>
       </c>
@@ -4271,16 +4276,16 @@
       <c r="G96" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H96" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="28"/>
-    </row>
-    <row r="97" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H96" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I96" s="25"/>
+      <c r="J96" s="25"/>
+      <c r="K96" s="25"/>
+      <c r="L96" s="25"/>
+      <c r="M96" s="25"/>
+    </row>
+    <row r="97" spans="1:13" ht="15.75" thickBot="1">
       <c r="A97" s="3" t="s">
         <v>117</v>
       </c>
@@ -4302,16 +4307,16 @@
       <c r="G97" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H97" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
-      <c r="M97" s="28"/>
-    </row>
-    <row r="98" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H97" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I97" s="25"/>
+      <c r="J97" s="25"/>
+      <c r="K97" s="25"/>
+      <c r="L97" s="25"/>
+      <c r="M97" s="25"/>
+    </row>
+    <row r="98" spans="1:13" ht="15.75" thickBot="1">
       <c r="A98" s="3" t="s">
         <v>119</v>
       </c>
@@ -4333,16 +4338,16 @@
       <c r="G98" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H98" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I98" s="28"/>
-      <c r="J98" s="28"/>
-      <c r="K98" s="28"/>
-      <c r="L98" s="28"/>
-      <c r="M98" s="28"/>
-    </row>
-    <row r="99" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H98" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I98" s="25"/>
+      <c r="J98" s="25"/>
+      <c r="K98" s="25"/>
+      <c r="L98" s="25"/>
+      <c r="M98" s="25"/>
+    </row>
+    <row r="99" spans="1:13" ht="15.75" thickBot="1">
       <c r="A99" s="3" t="s">
         <v>122</v>
       </c>
@@ -4364,16 +4369,16 @@
       <c r="G99" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H99" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
-      <c r="K99" s="28"/>
-      <c r="L99" s="28"/>
-      <c r="M99" s="28"/>
-    </row>
-    <row r="100" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H99" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I99" s="25"/>
+      <c r="J99" s="25"/>
+      <c r="K99" s="25"/>
+      <c r="L99" s="25"/>
+      <c r="M99" s="25"/>
+    </row>
+    <row r="100" spans="1:13" ht="15.75" thickBot="1">
       <c r="A100" s="3" t="s">
         <v>220</v>
       </c>
@@ -4395,16 +4400,16 @@
       <c r="G100" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H100" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-    </row>
-    <row r="101" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H100" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="25"/>
+      <c r="M100" s="25"/>
+    </row>
+    <row r="101" spans="1:13" ht="15.75" thickBot="1">
       <c r="A101" s="3" t="s">
         <v>222</v>
       </c>
@@ -4426,16 +4431,16 @@
       <c r="G101" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H101" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
-    </row>
-    <row r="102" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H101" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I101" s="25"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="25"/>
+      <c r="L101" s="25"/>
+      <c r="M101" s="25"/>
+    </row>
+    <row r="102" spans="1:13" ht="23.25" thickBot="1">
       <c r="A102" s="3" t="s">
         <v>224</v>
       </c>
@@ -4457,16 +4462,16 @@
       <c r="G102" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H102" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
-      <c r="K102" s="28"/>
-      <c r="L102" s="28"/>
-      <c r="M102" s="28"/>
-    </row>
-    <row r="103" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H102" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I102" s="25"/>
+      <c r="J102" s="25"/>
+      <c r="K102" s="25"/>
+      <c r="L102" s="25"/>
+      <c r="M102" s="25"/>
+    </row>
+    <row r="103" spans="1:13" ht="15.75" thickBot="1">
       <c r="A103" s="3" t="s">
         <v>226</v>
       </c>
@@ -4488,16 +4493,16 @@
       <c r="G103" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H103" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
-      <c r="K103" s="28"/>
-      <c r="L103" s="28"/>
-      <c r="M103" s="28"/>
-    </row>
-    <row r="104" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H103" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I103" s="25"/>
+      <c r="J103" s="25"/>
+      <c r="K103" s="25"/>
+      <c r="L103" s="25"/>
+      <c r="M103" s="25"/>
+    </row>
+    <row r="104" spans="1:13" ht="23.25" thickBot="1">
       <c r="A104" s="3" t="s">
         <v>228</v>
       </c>
@@ -4519,16 +4524,16 @@
       <c r="G104" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H104" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="28"/>
-      <c r="L104" s="28"/>
-      <c r="M104" s="28"/>
-    </row>
-    <row r="105" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H104" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I104" s="25"/>
+      <c r="J104" s="25"/>
+      <c r="K104" s="25"/>
+      <c r="L104" s="25"/>
+      <c r="M104" s="25"/>
+    </row>
+    <row r="105" spans="1:13" ht="15.75" thickBot="1">
       <c r="A105" s="3" t="s">
         <v>230</v>
       </c>
@@ -4550,16 +4555,16 @@
       <c r="G105" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H105" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="28"/>
-      <c r="L105" s="28"/>
-      <c r="M105" s="28"/>
-    </row>
-    <row r="106" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H105" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I105" s="25"/>
+      <c r="J105" s="25"/>
+      <c r="K105" s="25"/>
+      <c r="L105" s="25"/>
+      <c r="M105" s="25"/>
+    </row>
+    <row r="106" spans="1:13" ht="15.75" thickBot="1">
       <c r="A106" s="3" t="s">
         <v>232</v>
       </c>
@@ -4581,16 +4586,16 @@
       <c r="G106" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H106" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I106" s="28"/>
-      <c r="J106" s="28"/>
-      <c r="K106" s="28"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="28"/>
-    </row>
-    <row r="107" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H106" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I106" s="25"/>
+      <c r="J106" s="25"/>
+      <c r="K106" s="25"/>
+      <c r="L106" s="25"/>
+      <c r="M106" s="25"/>
+    </row>
+    <row r="107" spans="1:13" ht="15.75" thickBot="1">
       <c r="A107" s="3" t="s">
         <v>234</v>
       </c>
@@ -4612,16 +4617,16 @@
       <c r="G107" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H107" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
-      <c r="M107" s="28"/>
-    </row>
-    <row r="108" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H107" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I107" s="25"/>
+      <c r="J107" s="25"/>
+      <c r="K107" s="25"/>
+      <c r="L107" s="25"/>
+      <c r="M107" s="25"/>
+    </row>
+    <row r="108" spans="1:13" ht="23.25" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>236</v>
       </c>
@@ -4643,16 +4648,16 @@
       <c r="G108" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H108" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I108" s="28"/>
-      <c r="J108" s="28"/>
-      <c r="K108" s="28"/>
-      <c r="L108" s="28"/>
-      <c r="M108" s="28"/>
-    </row>
-    <row r="109" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H108" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I108" s="25"/>
+      <c r="J108" s="25"/>
+      <c r="K108" s="25"/>
+      <c r="L108" s="25"/>
+      <c r="M108" s="25"/>
+    </row>
+    <row r="109" spans="1:13" ht="23.25" thickBot="1">
       <c r="A109" s="3" t="s">
         <v>8</v>
       </c>
@@ -4674,16 +4679,16 @@
       <c r="G109" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H109" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I109" s="28"/>
-      <c r="J109" s="28"/>
-      <c r="K109" s="28"/>
-      <c r="L109" s="28"/>
-      <c r="M109" s="28"/>
-    </row>
-    <row r="110" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H109" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I109" s="25"/>
+      <c r="J109" s="25"/>
+      <c r="K109" s="25"/>
+      <c r="L109" s="25"/>
+      <c r="M109" s="25"/>
+    </row>
+    <row r="110" spans="1:13" ht="34.5" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>239</v>
       </c>
@@ -4705,16 +4710,16 @@
       <c r="G110" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H110" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I110" s="28"/>
-      <c r="J110" s="28"/>
-      <c r="K110" s="28"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="28"/>
-    </row>
-    <row r="111" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H110" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I110" s="25"/>
+      <c r="J110" s="25"/>
+      <c r="K110" s="25"/>
+      <c r="L110" s="25"/>
+      <c r="M110" s="25"/>
+    </row>
+    <row r="111" spans="1:13" ht="34.5" thickBot="1">
       <c r="A111" s="3" t="s">
         <v>241</v>
       </c>
@@ -4736,16 +4741,16 @@
       <c r="G111" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H111" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I111" s="28"/>
-      <c r="J111" s="28"/>
-      <c r="K111" s="28"/>
-      <c r="L111" s="28"/>
-      <c r="M111" s="28"/>
-    </row>
-    <row r="112" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H111" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I111" s="25"/>
+      <c r="J111" s="25"/>
+      <c r="K111" s="25"/>
+      <c r="L111" s="25"/>
+      <c r="M111" s="25"/>
+    </row>
+    <row r="112" spans="1:13" ht="34.5" thickBot="1">
       <c r="A112" s="3" t="s">
         <v>243</v>
       </c>
@@ -4767,16 +4772,16 @@
       <c r="G112" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H112" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I112" s="28"/>
-      <c r="J112" s="28"/>
-      <c r="K112" s="28"/>
-      <c r="L112" s="28"/>
-      <c r="M112" s="28"/>
-    </row>
-    <row r="113" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H112" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I112" s="25"/>
+      <c r="J112" s="25"/>
+      <c r="K112" s="25"/>
+      <c r="L112" s="25"/>
+      <c r="M112" s="25"/>
+    </row>
+    <row r="113" spans="1:13" ht="34.5" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>245</v>
       </c>
@@ -4798,16 +4803,16 @@
       <c r="G113" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H113" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I113" s="28"/>
-      <c r="J113" s="28"/>
-      <c r="K113" s="28"/>
-      <c r="L113" s="28"/>
-      <c r="M113" s="28"/>
-    </row>
-    <row r="114" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H113" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I113" s="25"/>
+      <c r="J113" s="25"/>
+      <c r="K113" s="25"/>
+      <c r="L113" s="25"/>
+      <c r="M113" s="25"/>
+    </row>
+    <row r="114" spans="1:13" ht="34.5" thickBot="1">
       <c r="A114" s="3" t="s">
         <v>247</v>
       </c>
@@ -4829,16 +4834,16 @@
       <c r="G114" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H114" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I114" s="28"/>
-      <c r="J114" s="28"/>
-      <c r="K114" s="28"/>
-      <c r="L114" s="28"/>
-      <c r="M114" s="28"/>
-    </row>
-    <row r="115" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H114" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I114" s="25"/>
+      <c r="J114" s="25"/>
+      <c r="K114" s="25"/>
+      <c r="L114" s="25"/>
+      <c r="M114" s="25"/>
+    </row>
+    <row r="115" spans="1:13" ht="34.5" thickBot="1">
       <c r="A115" s="3" t="s">
         <v>249</v>
       </c>
@@ -4860,20 +4865,21 @@
       <c r="G115" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H115" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="I115" s="28"/>
-      <c r="J115" s="28"/>
-      <c r="K115" s="28"/>
-      <c r="L115" s="28"/>
-      <c r="M115" s="28"/>
+      <c r="H115" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I115" s="25"/>
+      <c r="J115" s="25"/>
+      <c r="K115" s="25"/>
+      <c r="L115" s="25"/>
+      <c r="M115" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A69:G69"/>
     <mergeCell ref="A91:G91"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>